<commit_message>
Update with GW7 data
</commit_message>
<xml_diff>
--- a/results/Defenders_analysis.xlsx
+++ b/results/Defenders_analysis.xlsx
@@ -38,7 +38,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -67,12 +67,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCECE6"/>
+        <fgColor rgb="0098D8C9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E5F5F9"/>
+        <fgColor rgb="00CCECE6"/>
       </patternFill>
     </fill>
     <fill>
@@ -82,22 +82,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0098D8C9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="0040AD75"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EFF2F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DA3B46"/>
       </patternFill>
     </fill>
     <fill>
@@ -124,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -132,15 +117,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -602,22 +584,22 @@
         <v>3.274922949159448</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>2.166666666666667</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.5303459446912915</v>
+        <v>-0.581237727262678</v>
       </c>
       <c r="H2" t="n">
-        <v>1.336981695395218</v>
+        <v>1.237804526624875</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.299076951647973</v>
+        <v>-1.537810478945433</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1252966775082725</v>
+        <v>0.087505879937474</v>
       </c>
       <c r="K2" s="3" t="b">
         <v>0</v>
@@ -631,7 +613,7 @@
         <v>7.9</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="3">
@@ -650,36 +632,36 @@
         <v>2.440180484428572</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>3.333333333333333</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>4.571428571428571</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.1869289398009464</v>
+        <v>0.3204496110873369</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9961995111912456</v>
+        <v>0.9223015308444459</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.4578805206717523</v>
+        <v>0.8478299786644597</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3331244227947867</v>
+        <v>0.2145255250756623</v>
       </c>
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="6" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L3" s="7" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M3" s="2" t="n">
         <v>5.5</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="4">
@@ -698,36 +680,36 @@
         <v>3.114290373978884</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>3.666666666666667</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>3.142857142857143</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005633340999833761</v>
+        <v>-0.1625621259952023</v>
       </c>
       <c r="H4" t="n">
-        <v>1.271403721184944</v>
+        <v>1.177091119998638</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01379881099669273</v>
+        <v>-0.4300989579812535</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4947620785001176</v>
+        <v>0.3410711848842857</v>
       </c>
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="L4" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Very small</t>
         </is>
       </c>
       <c r="M4" s="2" t="n">
         <v>6.6</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="5">
@@ -746,36 +728,36 @@
         <v>3.064155175848397</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>1.666666666666667</v>
+        <v>2.285714285714286</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.5811395481604249</v>
+        <v>-0.3791107397218254</v>
       </c>
       <c r="H5" t="n">
-        <v>1.250936112256106</v>
+        <v>1.158141796258035</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.423495362344611</v>
+        <v>-1.003032736657686</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1069417678269359</v>
+        <v>0.1772831359460908</v>
       </c>
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="4" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L5" s="7" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="6">
@@ -794,7 +776,7 @@
         <v>2.390221306644396</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0</v>
@@ -803,13 +785,13 @@
         <v>-1.401543861519261</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9758037622678755</v>
+        <v>0.9034187365412755</v>
       </c>
       <c r="I6" t="n">
-        <v>-3.433067312852157</v>
+        <v>-3.708136509129114</v>
       </c>
       <c r="J6" t="n">
-        <v>0.009286944712771614</v>
+        <v>0.004995807688923841</v>
       </c>
       <c r="K6" s="3" t="b">
         <v>0</v>
@@ -823,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="7">
@@ -842,36 +824,36 @@
         <v>3.006050706846164</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>4.333333333333333</v>
+        <v>7</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3676794790512158</v>
+        <v>0.5894544029233778</v>
       </c>
       <c r="H7" t="n">
-        <v>1.227215062117634</v>
+        <v>1.136180371252125</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9006271125678155</v>
+        <v>1.559549759347322</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2045339180500253</v>
+        <v>0.08494144544397937</v>
       </c>
       <c r="K7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="10" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L7" s="4" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M7" s="2" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="N7" s="11" t="n">
-        <v>3.333333333333333</v>
+        <v>6.7</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="8">
@@ -890,36 +872,36 @@
         <v>2.264356756796147</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>4.333333333333333</v>
+        <v>7</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>3.714285714285714</v>
       </c>
       <c r="G8" t="n">
-        <v>0.507483109085445</v>
+        <v>0.2340952618791095</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9244197749623244</v>
+        <v>0.8558464082873387</v>
       </c>
       <c r="I8" t="n">
-        <v>1.243074670340514</v>
+        <v>0.6193578460306625</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1344754437242291</v>
+        <v>0.2792249342239432</v>
       </c>
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="4" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L8" s="7" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M8" s="2" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="N8" s="11" t="n">
-        <v>3.333333333333333</v>
+        <v>4.7</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="9">
@@ -938,36 +920,36 @@
         <v>3.57483031271498</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>3.166666666666667</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>3.285714285714286</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.002742485855554252</v>
+        <v>0.0305591281047475</v>
       </c>
       <c r="H9" t="n">
-        <v>1.459418363864287</v>
+        <v>1.351158855242728</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.006717690972908088</v>
+        <v>0.08085185324812649</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4974499425819603</v>
+        <v>0.4690946216569824</v>
       </c>
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Very small</t>
         </is>
       </c>
       <c r="M9" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N9" s="12" t="n">
-        <v>3</v>
+      <c r="N9" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="10">
@@ -986,27 +968,27 @@
         <v>3.172676002347705</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>3.666666666666667</v>
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>2.857142857142857</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1663509849058759</v>
+        <v>-0.08880390923546755</v>
       </c>
       <c r="H10" t="n">
-        <v>1.295239554154174</v>
+        <v>1.199158813256372</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4074750312288221</v>
+        <v>-0.2349530592873992</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3502593544435421</v>
+        <v>0.4110291563485409</v>
       </c>
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="6" t="inlineStr">
+      <c r="L10" s="8" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -1015,7 +997,7 @@
         <v>5.3</v>
       </c>
       <c r="N10" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="11">
@@ -1034,7 +1016,7 @@
         <v>3.121324107262869</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
@@ -1043,18 +1025,18 @@
         <v>-0.9526995942545613</v>
       </c>
       <c r="H11" t="n">
-        <v>1.27427523077371</v>
+        <v>1.179749621292607</v>
       </c>
       <c r="I11" t="n">
-        <v>-2.333627884080243</v>
+        <v>-2.520606200549709</v>
       </c>
       <c r="J11" t="n">
-        <v>0.03345423622211899</v>
+        <v>0.02262501373334546</v>
       </c>
       <c r="K11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="13" t="inlineStr">
+      <c r="L11" s="10" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
@@ -1063,7 +1045,7 @@
         <v>4.2</v>
       </c>
       <c r="N11" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="12">
@@ -1082,36 +1064,36 @@
         <v>2.401753745210275</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>2.166666666666667</v>
+        <v>1.857142857142857</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.2593134366026907</v>
+        <v>-0.3881875187774685</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9805118605972751</v>
+        <v>0.9077775886063392</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.6351856031241468</v>
+        <v>-1.027047636744398</v>
       </c>
       <c r="J12" t="n">
-        <v>0.276617240531838</v>
+        <v>0.1720047735946087</v>
       </c>
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="10" t="inlineStr">
+      <c r="L12" s="7" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
       </c>
       <c r="M12" s="2" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="N12" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="13">
@@ -1130,36 +1112,36 @@
         <v>2.385335314249029</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <v>2.833333333333333</v>
+        <v>7</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>3.285714285714286</v>
       </c>
       <c r="G13" t="n">
-        <v>0.04045185072881617</v>
+        <v>0.2301027353145644</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9738090642252475</v>
+        <v>0.9015720050004334</v>
       </c>
       <c r="I13" t="n">
-        <v>0.09908639343683143</v>
+        <v>0.6087946136380574</v>
       </c>
       <c r="J13" t="n">
-        <v>0.4624598279724852</v>
+        <v>0.2824911284356564</v>
       </c>
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="6" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L13" s="7" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M13" s="2" t="n">
         <v>4.5</v>
       </c>
-      <c r="N13" s="12" t="n">
-        <v>3</v>
+      <c r="N13" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="14">
@@ -1178,36 +1160,36 @@
         <v>2.64015602706141</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>1.666666666666667</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.3754429889807352</v>
+        <v>-0.5738439616658773</v>
       </c>
       <c r="H14" t="n">
-        <v>1.077839184605685</v>
+        <v>0.9978851814304007</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.9196437505081686</v>
+        <v>-1.518248413923994</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1999762526202849</v>
+        <v>0.08987562669715107</v>
       </c>
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L14" s="10" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L14" s="4" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M14" s="2" t="n">
         <v>5</v>
       </c>
       <c r="N14" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="15">
@@ -1226,27 +1208,27 @@
         <v>3.28177798758842</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>1.166666666666667</v>
+        <v>1.428571428571429</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.4410317902449626</v>
+        <v>-0.3612260377244456</v>
       </c>
       <c r="H15" t="n">
-        <v>1.339780253114909</v>
+        <v>1.240395487612139</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.080302846446338</v>
+        <v>-0.9557142629001192</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1646691617681293</v>
+        <v>0.1880605347805518</v>
       </c>
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="10" t="inlineStr">
+      <c r="L15" s="7" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
@@ -1255,7 +1237,7 @@
         <v>6</v>
       </c>
       <c r="N15" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="16">
@@ -1274,22 +1256,22 @@
         <v>3.023532400314094</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.5</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.6991937931605052</v>
+        <v>-0.7228180054961003</v>
       </c>
       <c r="H16" t="n">
-        <v>1.234351933590329</v>
+        <v>1.14278783031104</v>
       </c>
       <c r="I16" t="n">
-        <v>-1.71266802456432</v>
+        <v>-1.9123966857024</v>
       </c>
       <c r="J16" t="n">
-        <v>0.07372453489282628</v>
+        <v>0.05218027172442759</v>
       </c>
       <c r="K16" s="3" t="b">
         <v>0</v>
@@ -1303,7 +1285,7 @@
         <v>4.9</v>
       </c>
       <c r="N16" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="17">
@@ -1322,7 +1304,7 @@
         <v>2.686311740176314</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>0</v>
@@ -1331,18 +1313,18 @@
         <v>-0.9665636304369337</v>
       </c>
       <c r="H17" t="n">
-        <v>1.096682175579985</v>
+        <v>1.015330401214241</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.36758769850254</v>
+        <v>-2.557286992455868</v>
       </c>
       <c r="J17" t="n">
-        <v>0.03207214490649965</v>
+        <v>0.02153287183968387</v>
       </c>
       <c r="K17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="13" t="inlineStr">
+      <c r="L17" s="10" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
@@ -1350,8 +1332,8 @@
       <c r="M17" s="2" t="n">
         <v>4.3</v>
       </c>
-      <c r="N17" s="11" t="n">
-        <v>3.333333333333333</v>
+      <c r="N17" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="18">
@@ -1370,7 +1352,7 @@
         <v>2.573149666886379</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>0</v>
@@ -1379,18 +1361,18 @@
         <v>-0.9920260806423131</v>
       </c>
       <c r="H18" t="n">
-        <v>1.050483952614023</v>
+        <v>0.9725591578185789</v>
       </c>
       <c r="I18" t="n">
-        <v>-2.429957709106744</v>
+        <v>-2.624654303469667</v>
       </c>
       <c r="J18" t="n">
-        <v>0.02969188143562559</v>
+        <v>0.01967009716524104</v>
       </c>
       <c r="K18" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="13" t="inlineStr">
+      <c r="L18" s="10" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
@@ -1398,8 +1380,8 @@
       <c r="M18" s="2" t="n">
         <v>4.3</v>
       </c>
-      <c r="N18" s="12" t="n">
-        <v>3</v>
+      <c r="N18" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="19">
@@ -1418,27 +1400,27 @@
         <v>2.756102880805134</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
-      </c>
-      <c r="F19" s="7" t="n">
-        <v>2.833333333333333</v>
+        <v>7</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>2.571428571428572</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1082128015293689</v>
+        <v>0.01318559346366262</v>
       </c>
       <c r="H19" t="n">
-        <v>1.125174289431224</v>
+        <v>1.041708972902725</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2650661473840208</v>
+        <v>0.03488580119365008</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4007695933160456</v>
+        <v>0.4866512193676893</v>
       </c>
       <c r="K19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="6" t="inlineStr">
+      <c r="L19" s="8" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -1447,7 +1429,7 @@
         <v>4.5</v>
       </c>
       <c r="N19" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="20">
@@ -1466,36 +1448,36 @@
         <v>2.485739142100154</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
-      </c>
-      <c r="F20" s="7" t="n">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>5.142857142857143</v>
       </c>
       <c r="G20" t="n">
-        <v>0.6034422416234223</v>
+        <v>1.063207759050792</v>
       </c>
       <c r="H20" t="n">
-        <v>1.014798755301498</v>
+        <v>0.9395210848822935</v>
       </c>
       <c r="I20" t="n">
-        <v>1.478125581218661</v>
+        <v>2.812983322442678</v>
       </c>
       <c r="J20" t="n">
-        <v>0.09971283225193153</v>
+        <v>0.01531782510212264</v>
       </c>
       <c r="K20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="4" t="inlineStr">
-        <is>
-          <t>Medium</t>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>Large</t>
         </is>
       </c>
       <c r="M20" s="2" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="N20" s="12" t="n">
-        <v>3</v>
+        <v>4.7</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="21">
@@ -1514,27 +1496,27 @@
         <v>2.695643008276537</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>2.166666666666667</v>
+        <v>2.142857142857143</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.1187751633333659</v>
+        <v>-0.1276077586497414</v>
       </c>
       <c r="H21" t="n">
-        <v>1.100491649829761</v>
+        <v>1.018857289044249</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.2909385442824763</v>
+        <v>-0.3376183947495672</v>
       </c>
       <c r="J21" t="n">
-        <v>0.3913902321301346</v>
+        <v>0.3735746849348847</v>
       </c>
       <c r="K21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="6" t="inlineStr">
+      <c r="L21" s="8" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -1543,7 +1525,7 @@
         <v>4.5</v>
       </c>
       <c r="N21" s="5" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update original dashboards with GW10 data
</commit_message>
<xml_diff>
--- a/results/Defenders_analysis.xlsx
+++ b/results/Defenders_analysis.xlsx
@@ -38,7 +38,7 @@
       <color rgb="00F1F1F1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -62,12 +62,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0065C2A3"/>
+        <fgColor rgb="0098D8C9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0098D8C9"/>
+        <fgColor rgb="00228A44"/>
       </patternFill>
     </fill>
     <fill>
@@ -77,17 +77,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00228A44"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="0040AD75"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="0065C2A3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0094BCA7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F2F1F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="003A855E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DA3B46"/>
       </patternFill>
     </fill>
   </fills>
@@ -109,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -117,10 +132,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -584,36 +602,36 @@
         <v>3.274922949159448</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.581237727262678</v>
+        <v>-0.3980273100056864</v>
       </c>
       <c r="H2" t="n">
-        <v>1.237804526624875</v>
+        <v>1.035621568089967</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.537810478945433</v>
+        <v>-1.258672870567896</v>
       </c>
       <c r="J2" t="n">
-        <v>0.087505879937474</v>
+        <v>0.1199083647414327</v>
       </c>
       <c r="K2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="4" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="M2" s="2" t="n">
         <v>7.9</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="3">
@@ -632,36 +650,36 @@
         <v>2.440180484428572</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>4.571428571428571</v>
+        <v>4.4</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3204496110873369</v>
+        <v>0.2501971963489594</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9223015308444459</v>
+        <v>0.7716528232687325</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8478299786644597</v>
+        <v>0.791193004651076</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2145255250756623</v>
+        <v>0.2245893132427939</v>
       </c>
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="7" t="inlineStr">
+      <c r="L3" s="4" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
       </c>
       <c r="M3" s="2" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="N3" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>5.6</v>
+      </c>
+      <c r="N3" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="4">
@@ -680,36 +698,36 @@
         <v>3.114290373978884</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>3.142857142857143</v>
+        <v>2.3</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.1625621259952023</v>
+        <v>-0.4332039228872148</v>
       </c>
       <c r="H4" t="n">
-        <v>1.177091119998638</v>
+        <v>0.9848250876910851</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.4300989579812535</v>
+        <v>-1.369911087643545</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3410711848842857</v>
+        <v>0.1019582684673221</v>
       </c>
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="8" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M4" s="2" t="n">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="5">
@@ -728,27 +746,27 @@
         <v>3.064155175848397</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>2.285714285714286</v>
+        <v>2.3</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.3791107397218254</v>
+        <v>-0.3744485364501654</v>
       </c>
       <c r="H5" t="n">
-        <v>1.158141796258035</v>
+        <v>0.9689709459874698</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.003032736657686</v>
+        <v>-1.184110241699103</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1772831359460908</v>
+        <v>0.1333490921716224</v>
       </c>
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L5" s="7" t="inlineStr">
+      <c r="L5" s="4" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
@@ -756,8 +774,8 @@
       <c r="M5" s="2" t="n">
         <v>4.7</v>
       </c>
-      <c r="N5" s="5" t="n">
-        <v>3.142857142857143</v>
+      <c r="N5" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="6">
@@ -776,7 +794,7 @@
         <v>2.390221306644396</v>
       </c>
       <c r="E6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0</v>
@@ -785,18 +803,18 @@
         <v>-1.401543861519261</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9034187365412755</v>
+        <v>0.7558543440860045</v>
       </c>
       <c r="I6" t="n">
-        <v>-3.708136509129114</v>
+        <v>-4.432070843028485</v>
       </c>
       <c r="J6" t="n">
-        <v>0.004995807688923841</v>
-      </c>
-      <c r="K6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="9" t="inlineStr">
+        <v>0.0008211130378344513</v>
+      </c>
+      <c r="K6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8" t="inlineStr">
         <is>
           <t>Very large</t>
         </is>
@@ -804,8 +822,8 @@
       <c r="M6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N6" s="5" t="n">
-        <v>3.142857142857143</v>
+      <c r="N6" s="9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -824,36 +842,36 @@
         <v>3.006050706846164</v>
       </c>
       <c r="E7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.489655687180905</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.950596699559299</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.548427240746572</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.07796353688392833</v>
+      </c>
+      <c r="K7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4" t="inlineStr">
+        <is>
+          <t>Small</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.5894544029233778</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.136180371252125</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.559549759347322</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.08494144544397937</v>
-      </c>
-      <c r="K7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>6.7</v>
-      </c>
       <c r="N7" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="8">
@@ -872,27 +890,27 @@
         <v>2.264356756796147</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>3.714285714285714</v>
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>2.6</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2340952618791095</v>
+        <v>-0.2580028630922949</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8558464082873387</v>
+        <v>0.716052478666778</v>
       </c>
       <c r="I8" t="n">
-        <v>0.6193578460306625</v>
+        <v>-0.8158766902162451</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2792249342239432</v>
+        <v>0.2178155580478094</v>
       </c>
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="7" t="inlineStr">
+      <c r="L8" s="4" t="inlineStr">
         <is>
           <t>Small</t>
         </is>
@@ -901,7 +919,7 @@
         <v>4.7</v>
       </c>
       <c r="N8" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="9">
@@ -920,36 +938,36 @@
         <v>3.57483031271498</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>3.285714285714286</v>
+        <v>3.7</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0305591281047475</v>
+        <v>0.1464487446865977</v>
       </c>
       <c r="H9" t="n">
-        <v>1.351158855242728</v>
+        <v>1.130460603679132</v>
       </c>
       <c r="I9" t="n">
-        <v>0.08085185324812649</v>
+        <v>0.4631115936821305</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4690946216569824</v>
+        <v>0.3271394089645832</v>
       </c>
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="8" t="inlineStr">
+      <c r="L9" s="10" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
       </c>
       <c r="M9" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="N9" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>5.2</v>
+      </c>
+      <c r="N9" s="9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -968,36 +986,36 @@
         <v>3.172676002347705</v>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>2.857142857142857</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.08880390923546755</v>
+        <v>-0.3589679147968901</v>
       </c>
       <c r="H10" t="n">
-        <v>1.199158813256372</v>
+        <v>1.003288244517647</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.2349530592873992</v>
+        <v>-1.135156217679432</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4110291563485409</v>
+        <v>0.1428179015048393</v>
       </c>
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L10" s="8" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L10" s="4" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M10" s="2" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="N10" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>5</v>
+      </c>
+      <c r="N10" s="11" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="11">
@@ -1016,7 +1034,7 @@
         <v>3.121324107262869</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
@@ -1025,18 +1043,18 @@
         <v>-0.9526995942545613</v>
       </c>
       <c r="H11" t="n">
-        <v>1.179749621292607</v>
+        <v>0.9870493494542379</v>
       </c>
       <c r="I11" t="n">
-        <v>-2.520606200549709</v>
+        <v>-3.012700643762679</v>
       </c>
       <c r="J11" t="n">
-        <v>0.02262501373334546</v>
-      </c>
-      <c r="K11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11" s="10" t="inlineStr">
+        <v>0.00732579136431977</v>
+      </c>
+      <c r="K11" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="12" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
@@ -1044,8 +1062,8 @@
       <c r="M11" s="2" t="n">
         <v>4.2</v>
       </c>
-      <c r="N11" s="5" t="n">
-        <v>3.142857142857143</v>
+      <c r="N11" s="9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -1064,36 +1082,36 @@
         <v>2.401753745210275</v>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>1.857142857142857</v>
+        <v>1.3</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.3881875187774685</v>
+        <v>-0.6201608666920688</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9077775886063392</v>
+        <v>0.7595012213704189</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.027047636744398</v>
+        <v>-1.96112085445099</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1720047735946087</v>
+        <v>0.04074872336160689</v>
       </c>
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="7" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L12" s="13" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
       <c r="M12" s="2" t="n">
-        <v>4.5</v>
+        <v>4.4</v>
       </c>
       <c r="N12" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="13">
@@ -1112,36 +1130,36 @@
         <v>2.385335314249029</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F13" s="6" t="n">
-        <v>3.285714285714286</v>
+        <v>3</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2301027353145644</v>
+        <v>0.1103232292604076</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9015720050004334</v>
+        <v>0.7543092576260424</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6087946136380574</v>
+        <v>0.3488726832878215</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2824911284356564</v>
+        <v>0.3676038358419995</v>
       </c>
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="7" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L13" s="10" t="inlineStr">
+        <is>
+          <t>Very small</t>
         </is>
       </c>
       <c r="M13" s="2" t="n">
         <v>4.5</v>
       </c>
-      <c r="N13" s="5" t="n">
-        <v>3.142857142857143</v>
+      <c r="N13" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="14">
@@ -1160,36 +1178,36 @@
         <v>2.64015602706141</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>1.142857142857143</v>
+        <v>1.8</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.5738439616658773</v>
+        <v>-0.3249409232063354</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9978851814304007</v>
+        <v>0.8348906423735198</v>
       </c>
       <c r="I14" t="n">
-        <v>-1.518248413923994</v>
+        <v>-1.027553422329884</v>
       </c>
       <c r="J14" t="n">
-        <v>0.08987562669715107</v>
+        <v>0.1654916689918385</v>
       </c>
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="L14" s="4" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Small</t>
         </is>
       </c>
       <c r="M14" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N14" s="5" t="n">
-        <v>3.142857142857143</v>
+      <c r="N14" s="11" t="n">
+        <v>3.4</v>
       </c>
     </row>
     <row r="15">
@@ -1208,36 +1226,36 @@
         <v>3.28177798758842</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>1.428571428571429</v>
+        <v>2.3</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.3612260377244456</v>
+        <v>-0.09569053388345258</v>
       </c>
       <c r="H15" t="n">
-        <v>1.240395487612139</v>
+        <v>1.03778932157832</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.9557142629001192</v>
+        <v>-0.3026000375892274</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1880605347805518</v>
+        <v>0.3845358259576346</v>
       </c>
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L15" s="7" t="inlineStr">
-        <is>
-          <t>Small</t>
+      <c r="L15" s="10" t="inlineStr">
+        <is>
+          <t>Very small</t>
         </is>
       </c>
       <c r="M15" s="2" t="n">
         <v>6</v>
       </c>
       <c r="N15" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="16">
@@ -1256,36 +1274,36 @@
         <v>3.023532400314094</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.3</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.7228180054961003</v>
+        <v>-0.7653415877001714</v>
       </c>
       <c r="H16" t="n">
-        <v>1.14278783031104</v>
+        <v>0.9561248964308535</v>
       </c>
       <c r="I16" t="n">
-        <v>-1.9123966857024</v>
+        <v>-2.420222605182051</v>
       </c>
       <c r="J16" t="n">
-        <v>0.05218027172442759</v>
+        <v>0.01929826910069859</v>
       </c>
       <c r="K16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L16" s="4" t="inlineStr">
+      <c r="L16" s="13" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
       <c r="M16" s="2" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="N16" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="17">
@@ -1304,36 +1322,36 @@
         <v>2.686311740176314</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.9665636304369337</v>
+        <v>-0.8921121075519266</v>
       </c>
       <c r="H17" t="n">
-        <v>1.015330401214241</v>
+        <v>0.8494863604207602</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.557286992455868</v>
+        <v>-2.821106188077188</v>
       </c>
       <c r="J17" t="n">
-        <v>0.02153287183968387</v>
+        <v>0.01000541754143768</v>
       </c>
       <c r="K17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="10" t="inlineStr">
+      <c r="L17" s="12" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
       </c>
       <c r="M17" s="2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="N17" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>4.2</v>
+      </c>
+      <c r="N17" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="18">
@@ -1352,7 +1370,7 @@
         <v>2.573149666886379</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>0</v>
@@ -1361,27 +1379,27 @@
         <v>-0.9920260806423131</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9725591578185789</v>
+        <v>0.8137013707864504</v>
       </c>
       <c r="I18" t="n">
-        <v>-2.624654303469667</v>
+        <v>-3.137061913119582</v>
       </c>
       <c r="J18" t="n">
-        <v>0.01967009716524104</v>
-      </c>
-      <c r="K18" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="10" t="inlineStr">
+        <v>0.005992297787717643</v>
+      </c>
+      <c r="K18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="12" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
       </c>
       <c r="M18" s="2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="N18" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>4.2</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1400,27 +1418,27 @@
         <v>2.756102880805134</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>2.571428571428572</v>
+        <v>2.7</v>
       </c>
       <c r="G19" t="n">
-        <v>0.01318559346366262</v>
+        <v>0.05983531378682751</v>
       </c>
       <c r="H19" t="n">
-        <v>1.041708972902725</v>
+        <v>0.8715562569095788</v>
       </c>
       <c r="I19" t="n">
-        <v>0.03488580119365008</v>
+        <v>0.1892158760772497</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4866512193676893</v>
+        <v>0.4270609710876154</v>
       </c>
       <c r="K19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L19" s="8" t="inlineStr">
+      <c r="L19" s="10" t="inlineStr">
         <is>
           <t>Very small</t>
         </is>
@@ -1428,8 +1446,8 @@
       <c r="M19" s="2" t="n">
         <v>4.5</v>
       </c>
-      <c r="N19" s="5" t="n">
-        <v>3.142857142857143</v>
+      <c r="N19" s="9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -1448,36 +1466,36 @@
         <v>2.485739142100154</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F20" s="6" t="n">
-        <v>5.142857142857143</v>
+        <v>4.5</v>
       </c>
       <c r="G20" t="n">
-        <v>1.063207759050792</v>
+        <v>0.8045896554978965</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9395210848822935</v>
+        <v>0.7860597358069431</v>
       </c>
       <c r="I20" t="n">
-        <v>2.812983322442678</v>
+        <v>2.54433589318357</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01531782510212264</v>
+        <v>0.01574299586222637</v>
       </c>
       <c r="K20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="10" t="inlineStr">
+      <c r="L20" s="12" t="inlineStr">
         <is>
           <t>Large</t>
         </is>
       </c>
       <c r="M20" s="2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="N20" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>4.9</v>
+      </c>
+      <c r="N20" s="7" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="21">
@@ -1496,36 +1514,36 @@
         <v>2.695643008276537</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
-      </c>
-      <c r="F21" s="3" t="n">
-        <v>2.142857142857143</v>
+        <v>10</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>3.4</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.1276077586497414</v>
+        <v>0.3387532740548871</v>
       </c>
       <c r="H21" t="n">
-        <v>1.018857289044249</v>
+        <v>0.8524371664861977</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.3376183947495672</v>
+        <v>1.071231910852666</v>
       </c>
       <c r="J21" t="n">
-        <v>0.3735746849348847</v>
+        <v>0.1559748620484911</v>
       </c>
       <c r="K21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="L21" s="8" t="inlineStr">
-        <is>
-          <t>Very small</t>
+      <c r="L21" s="4" t="inlineStr">
+        <is>
+          <t>Small</t>
         </is>
       </c>
       <c r="M21" s="2" t="n">
         <v>4.5</v>
       </c>
       <c r="N21" s="5" t="n">
-        <v>3.142857142857143</v>
+        <v>3.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>